<commit_message>
se agrego la funcion para eliminar operario y se arreglo un problema en las fotos del informa calidad y con los precios
</commit_message>
<xml_diff>
--- a/server/doc/informeCalidad/FORMATO INFORME LIMON TAHITI.xlsx
+++ b/server/doc/informeCalidad/FORMATO INFORME LIMON TAHITI.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="5xfzmvwm1U3X4zmKnOwYlkwIEoPieIMc7pj8bTaMmKk="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="BWEnfDIYynAVYQISgcxclv18IdF82R4Of1RkUVzcZWk="/>
     </ext>
   </extLst>
 </workbook>
@@ -920,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1038,6 +1038,9 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="22" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -2525,7 +2528,7 @@
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G34" s="36"/>
+      <c r="G34" s="49"/>
       <c r="H34" s="44">
         <f>$E$34*$G$34</f>
         <v>0</v>
@@ -2628,15 +2631,15 @@
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="16"/>
-      <c r="E37" s="49">
+      <c r="E37" s="50">
         <f t="shared" ref="E37:F37" si="4">SUM(E17:E36)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="50" t="str">
+      <c r="F37" s="51" t="str">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G37" s="51"/>
+      <c r="G37" s="52"/>
       <c r="H37" s="44">
         <f>SUM(H17:H36)</f>
         <v>0</v>
@@ -2661,22 +2664,22 @@
       <c r="Z37" s="6"/>
     </row>
     <row r="38" ht="27.0" customHeight="1">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="55">
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="56">
         <f>E13+E37+E14</f>
         <v>0</v>
       </c>
-      <c r="F38" s="56" t="str">
+      <c r="F38" s="57" t="str">
         <f>SUM(F13+F37+F14)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G38" s="57"/>
-      <c r="H38" s="58">
+      <c r="G38" s="58"/>
+      <c r="H38" s="59">
         <f>$H$13+$H$37+$H$14</f>
         <v>0</v>
       </c>
@@ -2706,16 +2709,16 @@
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
       <c r="D39" s="30"/>
-      <c r="E39" s="59" t="s">
+      <c r="E39" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="F39" s="59" t="s">
+      <c r="F39" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="59" t="s">
+      <c r="G39" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="60" t="s">
+      <c r="H39" s="61" t="s">
         <v>21</v>
       </c>
       <c r="I39" s="6"/>
@@ -2745,7 +2748,7 @@
       <c r="E40" s="34">
         <v>0.0</v>
       </c>
-      <c r="F40" s="50"/>
+      <c r="F40" s="51"/>
       <c r="G40" s="36"/>
       <c r="H40" s="37">
         <f>+$E$40*$G$40</f>
@@ -2775,11 +2778,11 @@
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="16"/>
-      <c r="E41" s="61">
+      <c r="E41" s="62">
         <v>0.0</v>
       </c>
-      <c r="F41" s="62"/>
-      <c r="G41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="37">
         <f>+$E$41*$G$41</f>
         <v>0</v>
@@ -2808,11 +2811,11 @@
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="16"/>
-      <c r="E42" s="61">
+      <c r="E42" s="62">
         <v>0.0</v>
       </c>
-      <c r="F42" s="62"/>
-      <c r="G42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="37">
         <f>+$E$42*$G$42</f>
         <v>0</v>
@@ -2837,19 +2840,19 @@
       <c r="Z42" s="6"/>
     </row>
     <row r="43" ht="18.75" customHeight="1">
-      <c r="A43" s="52" t="s">
+      <c r="A43" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="55">
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="56">
         <f>$E$38+$E$40+$E$41+$E$42</f>
         <v>0</v>
       </c>
-      <c r="F43" s="56"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="58">
+      <c r="F43" s="57"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="59">
         <f>+$H$38+$H$40+$H$41+$H$42</f>
         <v>0</v>
       </c>
@@ -2873,14 +2876,14 @@
       <c r="Z43" s="6"/>
     </row>
     <row r="44" ht="12.0" customHeight="1">
-      <c r="A44" s="64"/>
-      <c r="B44" s="65"/>
-      <c r="C44" s="65"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="65"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="65"/>
+      <c r="A44" s="65"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -2901,16 +2904,16 @@
       <c r="Z44" s="6"/>
     </row>
     <row r="45" ht="24.0" customHeight="1">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="67"/>
+      <c r="B45" s="66"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="66"/>
+      <c r="F45" s="66"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="68"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -2931,28 +2934,28 @@
       <c r="Z45" s="6"/>
     </row>
     <row r="46" ht="26.25" customHeight="1">
-      <c r="A46" s="68" t="s">
+      <c r="A46" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="69">
+      <c r="B46" s="70">
         <v>0.0</v>
       </c>
-      <c r="C46" s="70" t="s">
+      <c r="C46" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="71">
+      <c r="D46" s="72">
         <v>0.0</v>
       </c>
-      <c r="E46" s="72" t="s">
+      <c r="E46" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="F46" s="69">
+      <c r="F46" s="70">
         <v>0.0</v>
       </c>
-      <c r="G46" s="70" t="s">
+      <c r="G46" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="H46" s="73">
+      <c r="H46" s="74">
         <v>0.0</v>
       </c>
       <c r="I46" s="6"/>
@@ -3087,16 +3090,16 @@
       <c r="Z50" s="6"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="52" t="s">
+      <c r="A51" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="74"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="75"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
@@ -3117,14 +3120,14 @@
       <c r="Z51" s="6"/>
     </row>
     <row r="52" ht="10.5" customHeight="1">
-      <c r="A52" s="75"/>
-      <c r="B52" s="76"/>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="76"/>
-      <c r="G52" s="76"/>
-      <c r="H52" s="76"/>
+      <c r="A52" s="76"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="77"/>
+      <c r="E52" s="77"/>
+      <c r="F52" s="77"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="77"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
@@ -3145,7 +3148,7 @@
       <c r="Z52" s="6"/>
     </row>
     <row r="53" ht="21.0" customHeight="1">
-      <c r="A53" s="77" t="s">
+      <c r="A53" s="78" t="s">
         <v>56</v>
       </c>
       <c r="I53" s="6"/>
@@ -3168,7 +3171,7 @@
       <c r="Z53" s="6"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="78"/>
+      <c r="A54" s="79"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -3189,16 +3192,16 @@
       <c r="Z54" s="6"/>
     </row>
     <row r="55" ht="18.75" customHeight="1">
-      <c r="A55" s="79" t="s">
+      <c r="A55" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="76"/>
-      <c r="C55" s="76"/>
-      <c r="D55" s="76"/>
-      <c r="E55" s="76"/>
-      <c r="F55" s="76"/>
-      <c r="G55" s="76"/>
-      <c r="H55" s="80"/>
+      <c r="B55" s="77"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="77"/>
+      <c r="E55" s="77"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="81"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -3219,18 +3222,18 @@
       <c r="Z55" s="6"/>
     </row>
     <row r="56" ht="16.5" customHeight="1">
-      <c r="A56" s="81" t="s">
+      <c r="A56" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="65"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="67"/>
-      <c r="E56" s="81" t="s">
+      <c r="B56" s="66"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="F56" s="65"/>
-      <c r="G56" s="65"/>
-      <c r="H56" s="67"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="68"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
@@ -3251,18 +3254,18 @@
       <c r="Z56" s="6"/>
     </row>
     <row r="57" ht="67.5" customHeight="1">
-      <c r="A57" s="82" t="s">
+      <c r="A57" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="65"/>
-      <c r="C57" s="65"/>
-      <c r="D57" s="67"/>
-      <c r="E57" s="82" t="s">
+      <c r="B57" s="66"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="F57" s="65"/>
-      <c r="G57" s="65"/>
-      <c r="H57" s="67"/>
+      <c r="F57" s="66"/>
+      <c r="G57" s="66"/>
+      <c r="H57" s="68"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
@@ -3283,18 +3286,18 @@
       <c r="Z57" s="6"/>
     </row>
     <row r="58" ht="24.0" customHeight="1">
-      <c r="A58" s="82" t="s">
+      <c r="A58" s="83" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="65"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="67"/>
-      <c r="E58" s="82" t="s">
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="F58" s="65"/>
-      <c r="G58" s="65"/>
-      <c r="H58" s="67"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="68"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
@@ -3315,18 +3318,18 @@
       <c r="Z58" s="6"/>
     </row>
     <row r="59" ht="70.5" customHeight="1">
-      <c r="A59" s="82" t="s">
+      <c r="A59" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B59" s="65"/>
-      <c r="C59" s="65"/>
-      <c r="D59" s="67"/>
-      <c r="E59" s="82" t="s">
+      <c r="B59" s="66"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="67"/>
+      <c r="F59" s="66"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="68"/>
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -3347,18 +3350,18 @@
       <c r="Z59" s="6"/>
     </row>
     <row r="60" ht="37.5" customHeight="1">
-      <c r="A60" s="82" t="s">
+      <c r="A60" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="65"/>
-      <c r="C60" s="65"/>
-      <c r="D60" s="67"/>
-      <c r="E60" s="82" t="s">
+      <c r="B60" s="66"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="68"/>
+      <c r="E60" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="F60" s="65"/>
-      <c r="G60" s="65"/>
-      <c r="H60" s="67"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="68"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -3379,18 +3382,18 @@
       <c r="Z60" s="6"/>
     </row>
     <row r="61" ht="39.75" customHeight="1">
-      <c r="A61" s="82" t="s">
+      <c r="A61" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="65"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="67"/>
-      <c r="E61" s="82" t="s">
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="68"/>
+      <c r="E61" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="F61" s="65"/>
-      <c r="G61" s="65"/>
-      <c r="H61" s="67"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="68"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -3411,14 +3414,14 @@
       <c r="Z61" s="6"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="83"/>
-      <c r="B62" s="83"/>
-      <c r="C62" s="83"/>
-      <c r="D62" s="83"/>
-      <c r="E62" s="83"/>
-      <c r="F62" s="83"/>
-      <c r="G62" s="83"/>
-      <c r="H62" s="83"/>
+      <c r="A62" s="84"/>
+      <c r="B62" s="84"/>
+      <c r="C62" s="84"/>
+      <c r="D62" s="84"/>
+      <c r="E62" s="84"/>
+      <c r="F62" s="84"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="84"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
@@ -3439,14 +3442,14 @@
       <c r="Z62" s="6"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="78"/>
-      <c r="B63" s="78"/>
-      <c r="C63" s="78"/>
-      <c r="D63" s="78"/>
-      <c r="E63" s="78"/>
-      <c r="F63" s="78"/>
-      <c r="G63" s="78"/>
-      <c r="H63" s="78"/>
+      <c r="A63" s="79"/>
+      <c r="B63" s="79"/>
+      <c r="C63" s="79"/>
+      <c r="D63" s="79"/>
+      <c r="E63" s="79"/>
+      <c r="F63" s="79"/>
+      <c r="G63" s="79"/>
+      <c r="H63" s="79"/>
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
       <c r="K63" s="6"/>
@@ -3467,14 +3470,14 @@
       <c r="Z63" s="6"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="78"/>
-      <c r="B64" s="78"/>
-      <c r="C64" s="78"/>
-      <c r="D64" s="78"/>
-      <c r="E64" s="78"/>
-      <c r="F64" s="78"/>
-      <c r="G64" s="78"/>
-      <c r="H64" s="78"/>
+      <c r="A64" s="79"/>
+      <c r="B64" s="79"/>
+      <c r="C64" s="79"/>
+      <c r="D64" s="79"/>
+      <c r="E64" s="79"/>
+      <c r="F64" s="79"/>
+      <c r="G64" s="79"/>
+      <c r="H64" s="79"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
@@ -3495,14 +3498,14 @@
       <c r="Z64" s="6"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="78"/>
-      <c r="B65" s="78"/>
-      <c r="C65" s="78"/>
-      <c r="D65" s="78"/>
-      <c r="E65" s="78"/>
-      <c r="F65" s="78"/>
-      <c r="G65" s="78"/>
-      <c r="H65" s="78"/>
+      <c r="A65" s="79"/>
+      <c r="B65" s="79"/>
+      <c r="C65" s="79"/>
+      <c r="D65" s="79"/>
+      <c r="E65" s="79"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="79"/>
+      <c r="H65" s="79"/>
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
@@ -3523,14 +3526,14 @@
       <c r="Z65" s="6"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="78"/>
-      <c r="B66" s="78"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
-      <c r="F66" s="78"/>
-      <c r="G66" s="78"/>
-      <c r="H66" s="78"/>
+      <c r="A66" s="79"/>
+      <c r="B66" s="79"/>
+      <c r="C66" s="79"/>
+      <c r="D66" s="79"/>
+      <c r="E66" s="79"/>
+      <c r="F66" s="79"/>
+      <c r="G66" s="79"/>
+      <c r="H66" s="79"/>
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
@@ -3551,14 +3554,14 @@
       <c r="Z66" s="6"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="78"/>
-      <c r="B67" s="78"/>
-      <c r="C67" s="78"/>
-      <c r="D67" s="78"/>
-      <c r="E67" s="78"/>
-      <c r="F67" s="78"/>
-      <c r="G67" s="78"/>
-      <c r="H67" s="78"/>
+      <c r="A67" s="79"/>
+      <c r="B67" s="79"/>
+      <c r="C67" s="79"/>
+      <c r="D67" s="79"/>
+      <c r="E67" s="79"/>
+      <c r="F67" s="79"/>
+      <c r="G67" s="79"/>
+      <c r="H67" s="79"/>
       <c r="I67" s="6"/>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
@@ -3579,14 +3582,14 @@
       <c r="Z67" s="6"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="78"/>
-      <c r="B68" s="78"/>
-      <c r="C68" s="78"/>
-      <c r="D68" s="78"/>
-      <c r="E68" s="78"/>
-      <c r="F68" s="78"/>
-      <c r="G68" s="78"/>
-      <c r="H68" s="78"/>
+      <c r="A68" s="79"/>
+      <c r="B68" s="79"/>
+      <c r="C68" s="79"/>
+      <c r="D68" s="79"/>
+      <c r="E68" s="79"/>
+      <c r="F68" s="79"/>
+      <c r="G68" s="79"/>
+      <c r="H68" s="79"/>
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
       <c r="K68" s="6"/>
@@ -3607,14 +3610,14 @@
       <c r="Z68" s="6"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="78"/>
-      <c r="B69" s="78"/>
-      <c r="C69" s="78"/>
-      <c r="D69" s="78"/>
-      <c r="E69" s="78"/>
-      <c r="F69" s="78"/>
-      <c r="G69" s="78"/>
-      <c r="H69" s="78"/>
+      <c r="A69" s="79"/>
+      <c r="B69" s="79"/>
+      <c r="C69" s="79"/>
+      <c r="D69" s="79"/>
+      <c r="E69" s="79"/>
+      <c r="F69" s="79"/>
+      <c r="G69" s="79"/>
+      <c r="H69" s="79"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -3635,14 +3638,14 @@
       <c r="Z69" s="6"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="78"/>
-      <c r="B70" s="78"/>
-      <c r="C70" s="78"/>
-      <c r="D70" s="78"/>
-      <c r="E70" s="78"/>
-      <c r="F70" s="78"/>
-      <c r="G70" s="78"/>
-      <c r="H70" s="78"/>
+      <c r="A70" s="79"/>
+      <c r="B70" s="79"/>
+      <c r="C70" s="79"/>
+      <c r="D70" s="79"/>
+      <c r="E70" s="79"/>
+      <c r="F70" s="79"/>
+      <c r="G70" s="79"/>
+      <c r="H70" s="79"/>
       <c r="I70" s="6"/>
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
@@ -3663,14 +3666,14 @@
       <c r="Z70" s="6"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="78"/>
-      <c r="B71" s="78"/>
-      <c r="C71" s="78"/>
-      <c r="D71" s="78"/>
-      <c r="E71" s="78"/>
-      <c r="F71" s="78"/>
-      <c r="G71" s="78"/>
-      <c r="H71" s="78"/>
+      <c r="A71" s="79"/>
+      <c r="B71" s="79"/>
+      <c r="C71" s="79"/>
+      <c r="D71" s="79"/>
+      <c r="E71" s="79"/>
+      <c r="F71" s="79"/>
+      <c r="G71" s="79"/>
+      <c r="H71" s="79"/>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
@@ -3691,14 +3694,16 @@
       <c r="Z71" s="6"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="78"/>
-      <c r="B72" s="78"/>
-      <c r="C72" s="78"/>
-      <c r="D72" s="78"/>
-      <c r="E72" s="78"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
-      <c r="H72" s="78"/>
+      <c r="A72" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="77"/>
+      <c r="C72" s="77"/>
+      <c r="D72" s="77"/>
+      <c r="E72" s="77"/>
+      <c r="F72" s="77"/>
+      <c r="G72" s="77"/>
+      <c r="H72" s="81"/>
       <c r="I72" s="6"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
@@ -3719,16 +3724,14 @@
       <c r="Z72" s="6"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="84" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="76"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
-      <c r="G73" s="76"/>
-      <c r="H73" s="80"/>
+      <c r="A73" s="86"/>
+      <c r="B73" s="77"/>
+      <c r="C73" s="77"/>
+      <c r="D73" s="77"/>
+      <c r="E73" s="81"/>
+      <c r="F73" s="86"/>
+      <c r="G73" s="77"/>
+      <c r="H73" s="81"/>
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
@@ -3749,14 +3752,10 @@
       <c r="Z73" s="6"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="85"/>
-      <c r="B74" s="76"/>
-      <c r="C74" s="76"/>
-      <c r="D74" s="76"/>
-      <c r="E74" s="80"/>
-      <c r="F74" s="85"/>
-      <c r="G74" s="76"/>
-      <c r="H74" s="80"/>
+      <c r="A74" s="87"/>
+      <c r="E74" s="88"/>
+      <c r="F74" s="87"/>
+      <c r="H74" s="88"/>
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
@@ -3777,10 +3776,10 @@
       <c r="Z74" s="6"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="86"/>
-      <c r="E75" s="87"/>
-      <c r="F75" s="86"/>
-      <c r="H75" s="87"/>
+      <c r="A75" s="87"/>
+      <c r="E75" s="88"/>
+      <c r="F75" s="87"/>
+      <c r="H75" s="88"/>
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
@@ -3801,10 +3800,10 @@
       <c r="Z75" s="6"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="86"/>
-      <c r="E76" s="87"/>
-      <c r="F76" s="86"/>
-      <c r="H76" s="87"/>
+      <c r="A76" s="87"/>
+      <c r="E76" s="88"/>
+      <c r="F76" s="87"/>
+      <c r="H76" s="88"/>
       <c r="I76" s="6"/>
       <c r="J76" s="6"/>
       <c r="K76" s="6"/>
@@ -3825,10 +3824,10 @@
       <c r="Z76" s="6"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="86"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="86"/>
-      <c r="H77" s="87"/>
+      <c r="A77" s="87"/>
+      <c r="E77" s="88"/>
+      <c r="F77" s="87"/>
+      <c r="H77" s="88"/>
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
       <c r="K77" s="6"/>
@@ -3849,10 +3848,10 @@
       <c r="Z77" s="6"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="86"/>
-      <c r="E78" s="87"/>
-      <c r="F78" s="86"/>
-      <c r="H78" s="87"/>
+      <c r="A78" s="87"/>
+      <c r="E78" s="88"/>
+      <c r="F78" s="87"/>
+      <c r="H78" s="88"/>
       <c r="I78" s="6"/>
       <c r="J78" s="6"/>
       <c r="K78" s="6"/>
@@ -3873,10 +3872,10 @@
       <c r="Z78" s="6"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="86"/>
-      <c r="E79" s="87"/>
-      <c r="F79" s="86"/>
-      <c r="H79" s="87"/>
+      <c r="A79" s="87"/>
+      <c r="E79" s="88"/>
+      <c r="F79" s="87"/>
+      <c r="H79" s="88"/>
       <c r="I79" s="6"/>
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
@@ -3897,10 +3896,10 @@
       <c r="Z79" s="6"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="86"/>
-      <c r="E80" s="87"/>
-      <c r="F80" s="86"/>
-      <c r="H80" s="87"/>
+      <c r="A80" s="87"/>
+      <c r="E80" s="88"/>
+      <c r="F80" s="87"/>
+      <c r="H80" s="88"/>
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
@@ -3921,10 +3920,10 @@
       <c r="Z80" s="6"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="86"/>
-      <c r="E81" s="87"/>
-      <c r="F81" s="86"/>
-      <c r="H81" s="87"/>
+      <c r="A81" s="87"/>
+      <c r="E81" s="88"/>
+      <c r="F81" s="87"/>
+      <c r="H81" s="88"/>
       <c r="I81" s="6"/>
       <c r="J81" s="6"/>
       <c r="K81" s="6"/>
@@ -3945,10 +3944,14 @@
       <c r="Z81" s="6"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="86"/>
-      <c r="E82" s="87"/>
-      <c r="F82" s="86"/>
-      <c r="H82" s="87"/>
+      <c r="A82" s="89"/>
+      <c r="B82" s="90"/>
+      <c r="C82" s="90"/>
+      <c r="D82" s="90"/>
+      <c r="E82" s="91"/>
+      <c r="F82" s="89"/>
+      <c r="G82" s="90"/>
+      <c r="H82" s="91"/>
       <c r="I82" s="6"/>
       <c r="J82" s="6"/>
       <c r="K82" s="6"/>
@@ -3969,14 +3972,14 @@
       <c r="Z82" s="6"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="88"/>
-      <c r="B83" s="89"/>
-      <c r="C83" s="89"/>
-      <c r="D83" s="89"/>
-      <c r="E83" s="90"/>
-      <c r="F83" s="88"/>
-      <c r="G83" s="89"/>
-      <c r="H83" s="90"/>
+      <c r="A83" s="92"/>
+      <c r="B83" s="66"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="66"/>
+      <c r="E83" s="68"/>
+      <c r="F83" s="92"/>
+      <c r="G83" s="66"/>
+      <c r="H83" s="68"/>
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
@@ -3997,14 +4000,14 @@
       <c r="Z83" s="6"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="91"/>
-      <c r="B84" s="65"/>
-      <c r="C84" s="65"/>
-      <c r="D84" s="65"/>
-      <c r="E84" s="67"/>
-      <c r="F84" s="91"/>
-      <c r="G84" s="65"/>
-      <c r="H84" s="67"/>
+      <c r="A84" s="86"/>
+      <c r="B84" s="77"/>
+      <c r="C84" s="77"/>
+      <c r="D84" s="77"/>
+      <c r="E84" s="81"/>
+      <c r="F84" s="86"/>
+      <c r="G84" s="77"/>
+      <c r="H84" s="81"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
@@ -4025,14 +4028,10 @@
       <c r="Z84" s="6"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="85"/>
-      <c r="B85" s="76"/>
-      <c r="C85" s="76"/>
-      <c r="D85" s="76"/>
-      <c r="E85" s="80"/>
-      <c r="F85" s="85"/>
-      <c r="G85" s="76"/>
-      <c r="H85" s="80"/>
+      <c r="A85" s="87"/>
+      <c r="E85" s="88"/>
+      <c r="F85" s="87"/>
+      <c r="H85" s="88"/>
       <c r="I85" s="6"/>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
@@ -4053,10 +4052,10 @@
       <c r="Z85" s="6"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="86"/>
-      <c r="E86" s="87"/>
-      <c r="F86" s="86"/>
-      <c r="H86" s="87"/>
+      <c r="A86" s="87"/>
+      <c r="E86" s="88"/>
+      <c r="F86" s="87"/>
+      <c r="H86" s="88"/>
       <c r="I86" s="6"/>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -4077,10 +4076,10 @@
       <c r="Z86" s="6"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="86"/>
-      <c r="E87" s="87"/>
-      <c r="F87" s="86"/>
-      <c r="H87" s="87"/>
+      <c r="A87" s="87"/>
+      <c r="E87" s="88"/>
+      <c r="F87" s="87"/>
+      <c r="H87" s="88"/>
       <c r="I87" s="6"/>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -4101,10 +4100,10 @@
       <c r="Z87" s="6"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="86"/>
-      <c r="E88" s="87"/>
-      <c r="F88" s="86"/>
-      <c r="H88" s="87"/>
+      <c r="A88" s="87"/>
+      <c r="E88" s="88"/>
+      <c r="F88" s="87"/>
+      <c r="H88" s="88"/>
       <c r="I88" s="6"/>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -4125,10 +4124,10 @@
       <c r="Z88" s="6"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="86"/>
-      <c r="E89" s="87"/>
-      <c r="F89" s="86"/>
-      <c r="H89" s="87"/>
+      <c r="A89" s="87"/>
+      <c r="E89" s="88"/>
+      <c r="F89" s="87"/>
+      <c r="H89" s="88"/>
       <c r="I89" s="6"/>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
@@ -4149,10 +4148,10 @@
       <c r="Z89" s="6"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="86"/>
-      <c r="E90" s="87"/>
-      <c r="F90" s="86"/>
-      <c r="H90" s="87"/>
+      <c r="A90" s="87"/>
+      <c r="E90" s="88"/>
+      <c r="F90" s="87"/>
+      <c r="H90" s="88"/>
       <c r="I90" s="6"/>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
@@ -4173,10 +4172,10 @@
       <c r="Z90" s="6"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="86"/>
-      <c r="E91" s="87"/>
-      <c r="F91" s="86"/>
-      <c r="H91" s="87"/>
+      <c r="A91" s="87"/>
+      <c r="E91" s="88"/>
+      <c r="F91" s="87"/>
+      <c r="H91" s="88"/>
       <c r="I91" s="6"/>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
@@ -4197,10 +4196,10 @@
       <c r="Z91" s="6"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="86"/>
-      <c r="E92" s="87"/>
-      <c r="F92" s="86"/>
-      <c r="H92" s="87"/>
+      <c r="A92" s="87"/>
+      <c r="E92" s="88"/>
+      <c r="F92" s="87"/>
+      <c r="H92" s="88"/>
       <c r="I92" s="6"/>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
@@ -4221,10 +4220,14 @@
       <c r="Z92" s="6"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="86"/>
-      <c r="E93" s="87"/>
-      <c r="F93" s="86"/>
-      <c r="H93" s="87"/>
+      <c r="A93" s="89"/>
+      <c r="B93" s="90"/>
+      <c r="C93" s="90"/>
+      <c r="D93" s="90"/>
+      <c r="E93" s="91"/>
+      <c r="F93" s="89"/>
+      <c r="G93" s="90"/>
+      <c r="H93" s="91"/>
       <c r="I93" s="6"/>
       <c r="J93" s="6"/>
       <c r="K93" s="6"/>
@@ -4245,14 +4248,14 @@
       <c r="Z93" s="6"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="88"/>
-      <c r="B94" s="89"/>
-      <c r="C94" s="89"/>
-      <c r="D94" s="89"/>
-      <c r="E94" s="90"/>
-      <c r="F94" s="88"/>
-      <c r="G94" s="89"/>
-      <c r="H94" s="90"/>
+      <c r="A94" s="92"/>
+      <c r="B94" s="66"/>
+      <c r="C94" s="66"/>
+      <c r="D94" s="66"/>
+      <c r="E94" s="68"/>
+      <c r="F94" s="92"/>
+      <c r="G94" s="66"/>
+      <c r="H94" s="68"/>
       <c r="I94" s="6"/>
       <c r="J94" s="6"/>
       <c r="K94" s="6"/>
@@ -4272,15 +4275,15 @@
       <c r="Y94" s="6"/>
       <c r="Z94" s="6"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="91"/>
-      <c r="B95" s="65"/>
-      <c r="C95" s="65"/>
-      <c r="D95" s="65"/>
-      <c r="E95" s="67"/>
-      <c r="F95" s="91"/>
-      <c r="G95" s="65"/>
-      <c r="H95" s="67"/>
+    <row r="95" ht="14.25" customHeight="1">
+      <c r="A95" s="86"/>
+      <c r="B95" s="77"/>
+      <c r="C95" s="77"/>
+      <c r="D95" s="77"/>
+      <c r="E95" s="81"/>
+      <c r="F95" s="86"/>
+      <c r="G95" s="77"/>
+      <c r="H95" s="81"/>
       <c r="I95" s="6"/>
       <c r="J95" s="6"/>
       <c r="K95" s="6"/>
@@ -4301,14 +4304,10 @@
       <c r="Z95" s="6"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="85"/>
-      <c r="B96" s="76"/>
-      <c r="C96" s="76"/>
-      <c r="D96" s="76"/>
-      <c r="E96" s="80"/>
-      <c r="F96" s="85"/>
-      <c r="G96" s="76"/>
-      <c r="H96" s="80"/>
+      <c r="A96" s="87"/>
+      <c r="E96" s="88"/>
+      <c r="F96" s="87"/>
+      <c r="H96" s="88"/>
       <c r="I96" s="6"/>
       <c r="J96" s="6"/>
       <c r="K96" s="6"/>
@@ -4329,10 +4328,10 @@
       <c r="Z96" s="6"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="86"/>
-      <c r="E97" s="87"/>
-      <c r="F97" s="86"/>
-      <c r="H97" s="87"/>
+      <c r="A97" s="87"/>
+      <c r="E97" s="88"/>
+      <c r="F97" s="87"/>
+      <c r="H97" s="88"/>
       <c r="I97" s="6"/>
       <c r="J97" s="6"/>
       <c r="K97" s="6"/>
@@ -4353,10 +4352,10 @@
       <c r="Z97" s="6"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="86"/>
-      <c r="E98" s="87"/>
-      <c r="F98" s="86"/>
-      <c r="H98" s="87"/>
+      <c r="A98" s="87"/>
+      <c r="E98" s="88"/>
+      <c r="F98" s="87"/>
+      <c r="H98" s="88"/>
       <c r="I98" s="6"/>
       <c r="J98" s="6"/>
       <c r="K98" s="6"/>
@@ -4377,10 +4376,10 @@
       <c r="Z98" s="6"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
-      <c r="A99" s="86"/>
-      <c r="E99" s="87"/>
-      <c r="F99" s="86"/>
-      <c r="H99" s="87"/>
+      <c r="A99" s="87"/>
+      <c r="E99" s="88"/>
+      <c r="F99" s="87"/>
+      <c r="H99" s="88"/>
       <c r="I99" s="6"/>
       <c r="J99" s="6"/>
       <c r="K99" s="6"/>
@@ -4401,10 +4400,10 @@
       <c r="Z99" s="6"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
-      <c r="A100" s="86"/>
-      <c r="E100" s="87"/>
-      <c r="F100" s="86"/>
-      <c r="H100" s="87"/>
+      <c r="A100" s="87"/>
+      <c r="E100" s="88"/>
+      <c r="F100" s="87"/>
+      <c r="H100" s="88"/>
       <c r="I100" s="6"/>
       <c r="J100" s="6"/>
       <c r="K100" s="6"/>
@@ -4425,10 +4424,10 @@
       <c r="Z100" s="6"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
-      <c r="A101" s="86"/>
-      <c r="E101" s="87"/>
-      <c r="F101" s="86"/>
-      <c r="H101" s="87"/>
+      <c r="A101" s="87"/>
+      <c r="E101" s="88"/>
+      <c r="F101" s="87"/>
+      <c r="H101" s="88"/>
       <c r="I101" s="6"/>
       <c r="J101" s="6"/>
       <c r="K101" s="6"/>
@@ -4449,10 +4448,10 @@
       <c r="Z101" s="6"/>
     </row>
     <row r="102" ht="14.25" customHeight="1">
-      <c r="A102" s="86"/>
-      <c r="E102" s="87"/>
-      <c r="F102" s="86"/>
-      <c r="H102" s="87"/>
+      <c r="A102" s="87"/>
+      <c r="E102" s="88"/>
+      <c r="F102" s="87"/>
+      <c r="H102" s="88"/>
       <c r="I102" s="6"/>
       <c r="J102" s="6"/>
       <c r="K102" s="6"/>
@@ -4473,10 +4472,10 @@
       <c r="Z102" s="6"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
-      <c r="A103" s="86"/>
-      <c r="E103" s="87"/>
-      <c r="F103" s="86"/>
-      <c r="H103" s="87"/>
+      <c r="A103" s="87"/>
+      <c r="E103" s="88"/>
+      <c r="F103" s="87"/>
+      <c r="H103" s="88"/>
       <c r="I103" s="6"/>
       <c r="J103" s="6"/>
       <c r="K103" s="6"/>
@@ -4496,11 +4495,15 @@
       <c r="Y103" s="6"/>
       <c r="Z103" s="6"/>
     </row>
-    <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="86"/>
-      <c r="E104" s="87"/>
-      <c r="F104" s="86"/>
-      <c r="H104" s="87"/>
+    <row r="104" ht="15.0" customHeight="1">
+      <c r="A104" s="89"/>
+      <c r="B104" s="90"/>
+      <c r="C104" s="90"/>
+      <c r="D104" s="90"/>
+      <c r="E104" s="91"/>
+      <c r="F104" s="89"/>
+      <c r="G104" s="90"/>
+      <c r="H104" s="91"/>
       <c r="I104" s="6"/>
       <c r="J104" s="6"/>
       <c r="K104" s="6"/>
@@ -4520,15 +4523,15 @@
       <c r="Y104" s="6"/>
       <c r="Z104" s="6"/>
     </row>
-    <row r="105" ht="15.0" customHeight="1">
-      <c r="A105" s="88"/>
-      <c r="B105" s="89"/>
-      <c r="C105" s="89"/>
-      <c r="D105" s="89"/>
-      <c r="E105" s="90"/>
-      <c r="F105" s="88"/>
-      <c r="G105" s="89"/>
-      <c r="H105" s="90"/>
+    <row r="105" ht="15.75" customHeight="1">
+      <c r="A105" s="92"/>
+      <c r="B105" s="66"/>
+      <c r="C105" s="66"/>
+      <c r="D105" s="66"/>
+      <c r="E105" s="68"/>
+      <c r="F105" s="92"/>
+      <c r="G105" s="66"/>
+      <c r="H105" s="68"/>
       <c r="I105" s="6"/>
       <c r="J105" s="6"/>
       <c r="K105" s="6"/>
@@ -4549,14 +4552,14 @@
       <c r="Z105" s="6"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="91"/>
-      <c r="B106" s="65"/>
-      <c r="C106" s="65"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="67"/>
-      <c r="F106" s="91"/>
-      <c r="G106" s="65"/>
-      <c r="H106" s="67"/>
+      <c r="A106" s="86"/>
+      <c r="B106" s="77"/>
+      <c r="C106" s="77"/>
+      <c r="D106" s="77"/>
+      <c r="E106" s="81"/>
+      <c r="F106" s="86"/>
+      <c r="G106" s="77"/>
+      <c r="H106" s="81"/>
       <c r="I106" s="6"/>
       <c r="J106" s="6"/>
       <c r="K106" s="6"/>
@@ -4577,14 +4580,10 @@
       <c r="Z106" s="6"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="85"/>
-      <c r="B107" s="76"/>
-      <c r="C107" s="76"/>
-      <c r="D107" s="76"/>
-      <c r="E107" s="80"/>
-      <c r="F107" s="85"/>
-      <c r="G107" s="76"/>
-      <c r="H107" s="80"/>
+      <c r="A107" s="87"/>
+      <c r="E107" s="88"/>
+      <c r="F107" s="87"/>
+      <c r="H107" s="88"/>
       <c r="I107" s="6"/>
       <c r="J107" s="6"/>
       <c r="K107" s="6"/>
@@ -4605,10 +4604,10 @@
       <c r="Z107" s="6"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="86"/>
-      <c r="E108" s="87"/>
-      <c r="F108" s="86"/>
-      <c r="H108" s="87"/>
+      <c r="A108" s="87"/>
+      <c r="E108" s="88"/>
+      <c r="F108" s="87"/>
+      <c r="H108" s="88"/>
       <c r="I108" s="6"/>
       <c r="J108" s="6"/>
       <c r="K108" s="6"/>
@@ -4629,10 +4628,10 @@
       <c r="Z108" s="6"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="86"/>
-      <c r="E109" s="87"/>
-      <c r="F109" s="86"/>
-      <c r="H109" s="87"/>
+      <c r="A109" s="87"/>
+      <c r="E109" s="88"/>
+      <c r="F109" s="87"/>
+      <c r="H109" s="88"/>
       <c r="I109" s="6"/>
       <c r="J109" s="6"/>
       <c r="K109" s="6"/>
@@ -4653,10 +4652,10 @@
       <c r="Z109" s="6"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="86"/>
-      <c r="E110" s="87"/>
-      <c r="F110" s="86"/>
-      <c r="H110" s="87"/>
+      <c r="A110" s="87"/>
+      <c r="E110" s="88"/>
+      <c r="F110" s="87"/>
+      <c r="H110" s="88"/>
       <c r="I110" s="6"/>
       <c r="J110" s="6"/>
       <c r="K110" s="6"/>
@@ -4677,10 +4676,10 @@
       <c r="Z110" s="6"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="86"/>
-      <c r="E111" s="87"/>
-      <c r="F111" s="86"/>
-      <c r="H111" s="87"/>
+      <c r="A111" s="87"/>
+      <c r="E111" s="88"/>
+      <c r="F111" s="87"/>
+      <c r="H111" s="88"/>
       <c r="I111" s="6"/>
       <c r="J111" s="6"/>
       <c r="K111" s="6"/>
@@ -4701,10 +4700,10 @@
       <c r="Z111" s="6"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="86"/>
-      <c r="E112" s="87"/>
-      <c r="F112" s="86"/>
-      <c r="H112" s="87"/>
+      <c r="A112" s="87"/>
+      <c r="E112" s="88"/>
+      <c r="F112" s="87"/>
+      <c r="H112" s="88"/>
       <c r="I112" s="6"/>
       <c r="J112" s="6"/>
       <c r="K112" s="6"/>
@@ -4725,10 +4724,10 @@
       <c r="Z112" s="6"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="86"/>
-      <c r="E113" s="87"/>
-      <c r="F113" s="86"/>
-      <c r="H113" s="87"/>
+      <c r="A113" s="87"/>
+      <c r="E113" s="88"/>
+      <c r="F113" s="87"/>
+      <c r="H113" s="88"/>
       <c r="I113" s="6"/>
       <c r="J113" s="6"/>
       <c r="K113" s="6"/>
@@ -4749,10 +4748,10 @@
       <c r="Z113" s="6"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="86"/>
-      <c r="E114" s="87"/>
-      <c r="F114" s="86"/>
-      <c r="H114" s="87"/>
+      <c r="A114" s="87"/>
+      <c r="E114" s="88"/>
+      <c r="F114" s="87"/>
+      <c r="H114" s="88"/>
       <c r="I114" s="6"/>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
@@ -4773,10 +4772,14 @@
       <c r="Z114" s="6"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="86"/>
-      <c r="E115" s="87"/>
-      <c r="F115" s="86"/>
-      <c r="H115" s="87"/>
+      <c r="A115" s="89"/>
+      <c r="B115" s="90"/>
+      <c r="C115" s="90"/>
+      <c r="D115" s="90"/>
+      <c r="E115" s="91"/>
+      <c r="F115" s="89"/>
+      <c r="G115" s="90"/>
+      <c r="H115" s="91"/>
       <c r="I115" s="6"/>
       <c r="J115" s="6"/>
       <c r="K115" s="6"/>
@@ -4797,14 +4800,14 @@
       <c r="Z115" s="6"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="88"/>
-      <c r="B116" s="89"/>
-      <c r="C116" s="89"/>
-      <c r="D116" s="89"/>
-      <c r="E116" s="90"/>
-      <c r="F116" s="88"/>
-      <c r="G116" s="89"/>
-      <c r="H116" s="90"/>
+      <c r="A116" s="92"/>
+      <c r="B116" s="66"/>
+      <c r="C116" s="66"/>
+      <c r="D116" s="66"/>
+      <c r="E116" s="68"/>
+      <c r="F116" s="92"/>
+      <c r="G116" s="66"/>
+      <c r="H116" s="68"/>
       <c r="I116" s="6"/>
       <c r="J116" s="6"/>
       <c r="K116" s="6"/>
@@ -4825,14 +4828,14 @@
       <c r="Z116" s="6"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="91"/>
-      <c r="B117" s="65"/>
-      <c r="C117" s="65"/>
-      <c r="D117" s="65"/>
-      <c r="E117" s="67"/>
-      <c r="F117" s="91"/>
-      <c r="G117" s="65"/>
-      <c r="H117" s="67"/>
+      <c r="A117" s="6"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
       <c r="I117" s="6"/>
       <c r="J117" s="6"/>
       <c r="K117" s="6"/>
@@ -29576,34 +29579,6 @@
       <c r="Y1000" s="6"/>
       <c r="Z1000" s="6"/>
     </row>
-    <row r="1001" ht="15.75" customHeight="1">
-      <c r="A1001" s="6"/>
-      <c r="B1001" s="6"/>
-      <c r="C1001" s="6"/>
-      <c r="D1001" s="6"/>
-      <c r="E1001" s="6"/>
-      <c r="F1001" s="6"/>
-      <c r="G1001" s="6"/>
-      <c r="H1001" s="6"/>
-      <c r="I1001" s="6"/>
-      <c r="J1001" s="6"/>
-      <c r="K1001" s="6"/>
-      <c r="L1001" s="6"/>
-      <c r="M1001" s="6"/>
-      <c r="N1001" s="6"/>
-      <c r="O1001" s="6"/>
-      <c r="P1001" s="6"/>
-      <c r="Q1001" s="6"/>
-      <c r="R1001" s="6"/>
-      <c r="S1001" s="6"/>
-      <c r="T1001" s="6"/>
-      <c r="U1001" s="6"/>
-      <c r="V1001" s="6"/>
-      <c r="W1001" s="6"/>
-      <c r="X1001" s="6"/>
-      <c r="Y1001" s="6"/>
-      <c r="Z1001" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="85">
     <mergeCell ref="A56:D56"/>
@@ -29624,23 +29599,23 @@
     <mergeCell ref="E59:H59"/>
     <mergeCell ref="E60:H60"/>
     <mergeCell ref="E61:H61"/>
-    <mergeCell ref="A73:H73"/>
-    <mergeCell ref="F74:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="A96:E105"/>
-    <mergeCell ref="A106:E106"/>
-    <mergeCell ref="A107:E116"/>
-    <mergeCell ref="F107:H116"/>
-    <mergeCell ref="A117:E117"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="A74:E83"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A85:E94"/>
-    <mergeCell ref="F85:H94"/>
-    <mergeCell ref="A95:E95"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F96:H105"/>
-    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="A72:H72"/>
+    <mergeCell ref="F73:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="A95:E104"/>
+    <mergeCell ref="A105:E105"/>
+    <mergeCell ref="A106:E115"/>
+    <mergeCell ref="F106:H115"/>
+    <mergeCell ref="A116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="A73:E82"/>
+    <mergeCell ref="A83:E83"/>
+    <mergeCell ref="A84:E93"/>
+    <mergeCell ref="F84:H93"/>
+    <mergeCell ref="A94:E94"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H104"/>
+    <mergeCell ref="F105:H105"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:G4"/>
     <mergeCell ref="H1:H4"/>

</xml_diff>